<commit_message>
use new meta define files for new data (unfinished with compiling errors)
</commit_message>
<xml_diff>
--- a/bin/resource/excel/entity_class.xlsx
+++ b/bin/resource/excel/entity_class.xlsx
@@ -24,7 +24,7 @@
     <author>1</author>
   </authors>
   <commentList>
-    <comment ref="C24" authorId="0" shapeId="0">
+    <comment ref="C25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="117">
   <si>
     <t>class</t>
   </si>
@@ -408,6 +408,47 @@
       </rPr>
       <t>32</t>
     </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ap_inst_id</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nt</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前副本id</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -850,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1226,23 +1267,23 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>113</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="E11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="3">
-        <v>1</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="J11" s="9">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9">
         <v>1</v>
       </c>
       <c r="L11">
@@ -1251,7 +1292,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="3">
+      <c r="P11" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1260,29 +1301,29 @@
         <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
         <v>1</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12">
+      <c r="P12" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1291,29 +1332,29 @@
         <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="3">
-        <v>1</v>
-      </c>
-      <c r="K13" s="3">
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
         <v>1</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="3">
+      <c r="P13">
         <v>0</v>
       </c>
     </row>
@@ -1322,20 +1363,20 @@
         <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3">
         <v>1</v>
       </c>
       <c r="L14">
@@ -1344,7 +1385,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14">
+      <c r="P14" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1353,20 +1394,20 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="3">
-        <v>1</v>
-      </c>
-      <c r="K15" s="3">
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
         <v>1</v>
       </c>
       <c r="L15">
@@ -1375,7 +1416,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="3">
+      <c r="P15">
         <v>0</v>
       </c>
     </row>
@@ -1384,20 +1425,20 @@
         <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
+      <c r="J16" s="3">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3">
         <v>1</v>
       </c>
       <c r="L16">
@@ -1406,7 +1447,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16">
+      <c r="P16" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1415,20 +1456,20 @@
         <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="3">
-        <v>1</v>
-      </c>
-      <c r="K17" s="3">
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
         <v>1</v>
       </c>
       <c r="L17">
@@ -1437,7 +1478,7 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="3">
+      <c r="P17">
         <v>0</v>
       </c>
     </row>
@@ -1446,20 +1487,20 @@
         <v>30</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="E18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18">
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
         <v>1</v>
       </c>
       <c r="L18">
@@ -1468,7 +1509,7 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18">
+      <c r="P18" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1477,20 +1518,20 @@
         <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>111</v>
+      <c r="D19" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="3">
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
         <v>1</v>
       </c>
       <c r="L19">
@@ -1499,7 +1540,7 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="3">
+      <c r="P19">
         <v>0</v>
       </c>
     </row>
@@ -1508,20 +1549,20 @@
         <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>65</v>
+      <c r="D20" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="E20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
+      <c r="J20" s="3">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3">
         <v>1</v>
       </c>
       <c r="L20">
@@ -1530,7 +1571,7 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20">
+      <c r="P20" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1539,20 +1580,20 @@
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="D21" t="s">
-        <v>67</v>
+      <c r="D21" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="E21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="3">
-        <v>1</v>
-      </c>
-      <c r="K21" s="3">
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
         <v>1</v>
       </c>
       <c r="L21">
@@ -1561,7 +1602,7 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="3">
+      <c r="P21">
         <v>0</v>
       </c>
     </row>
@@ -1570,20 +1611,20 @@
         <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
         <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
+      <c r="J22" s="3">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3">
         <v>1</v>
       </c>
       <c r="L22">
@@ -1592,7 +1633,7 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22">
+      <c r="P22" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1601,20 +1642,20 @@
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="3">
-        <v>1</v>
-      </c>
-      <c r="K23" s="3">
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
         <v>1</v>
       </c>
       <c r="L23">
@@ -1623,7 +1664,7 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-      <c r="P23" s="3">
+      <c r="P23">
         <v>0</v>
       </c>
     </row>
@@ -1631,24 +1672,21 @@
       <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="s">
-        <v>72</v>
+      <c r="B24" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="G24" t="s">
-        <v>75</v>
-      </c>
       <c r="I24" s="4"/>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="K24">
+      <c r="J24" s="3">
+        <v>1</v>
+      </c>
+      <c r="K24" s="3">
         <v>1</v>
       </c>
       <c r="L24">
@@ -1657,7 +1695,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-      <c r="P24">
+      <c r="P24" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1666,23 +1704,23 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E25" s="4"/>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="3">
-        <v>1</v>
-      </c>
-      <c r="K25" s="3">
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
         <v>1</v>
       </c>
       <c r="L25">
@@ -1691,7 +1729,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-      <c r="P25" s="3">
+      <c r="P25">
         <v>0</v>
       </c>
     </row>
@@ -1700,23 +1738,23 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
         <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E26" s="4"/>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="K26">
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3">
         <v>1</v>
       </c>
       <c r="L26">
@@ -1725,24 +1763,27 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
-      <c r="P26">
+      <c r="P26" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E27" s="4"/>
+      <c r="G27" t="s">
+        <v>82</v>
+      </c>
       <c r="I27" s="4"/>
       <c r="J27">
         <v>1</v>
@@ -1756,7 +1797,7 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-      <c r="P27" s="3">
+      <c r="P27">
         <v>0</v>
       </c>
     </row>
@@ -1764,21 +1805,21 @@
       <c r="A28" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>112</v>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E28" s="4"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="3">
-        <v>1</v>
-      </c>
-      <c r="K28" s="3">
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
         <v>1</v>
       </c>
       <c r="L28">
@@ -1787,7 +1828,7 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28">
+      <c r="P28" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1796,20 +1837,20 @@
         <v>79</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
+        <v>85</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="K29">
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3">
         <v>1</v>
       </c>
       <c r="L29">
@@ -1818,7 +1859,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29" s="3">
+      <c r="P29">
         <v>0</v>
       </c>
     </row>
@@ -1827,20 +1868,20 @@
         <v>79</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="3">
-        <v>1</v>
-      </c>
-      <c r="K30" s="3">
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
         <v>1</v>
       </c>
       <c r="L30">
@@ -1849,7 +1890,7 @@
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-      <c r="P30">
+      <c r="P30" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1858,20 +1899,20 @@
         <v>79</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E31" s="4"/>
       <c r="I31" s="4"/>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31">
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3">
         <v>1</v>
       </c>
       <c r="L31">
@@ -1880,7 +1921,7 @@
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-      <c r="P31" s="3">
+      <c r="P31">
         <v>0</v>
       </c>
     </row>
@@ -1889,13 +1930,13 @@
         <v>79</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
         <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E32" s="4"/>
       <c r="I32" s="4"/>
@@ -1911,22 +1952,22 @@
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
-      <c r="P32">
+      <c r="P32" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="4"/>
       <c r="I33" s="4"/>
@@ -1942,7 +1983,7 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="3">
+      <c r="P33">
         <v>0</v>
       </c>
     </row>
@@ -1951,13 +1992,13 @@
         <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>112</v>
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
       </c>
       <c r="D34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="4"/>
       <c r="I34" s="4"/>
@@ -1968,32 +2009,32 @@
         <v>1</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34">
+      <c r="P34" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" t="s">
-        <v>99</v>
+        <v>85</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -2004,7 +2045,7 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="3">
+      <c r="P35">
         <v>0</v>
       </c>
     </row>
@@ -2013,13 +2054,13 @@
         <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
         <v>99</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E36" s="4"/>
       <c r="I36" s="4"/>
@@ -2035,7 +2076,7 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36">
+      <c r="P36" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2044,13 +2085,13 @@
         <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C37" t="s">
         <v>99</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E37" s="4"/>
       <c r="I37" s="4"/>
@@ -2066,7 +2107,7 @@
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
-      <c r="P37" s="3">
+      <c r="P37">
         <v>0</v>
       </c>
     </row>
@@ -2075,13 +2116,13 @@
         <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
         <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E38" s="4"/>
       <c r="I38" s="4"/>
@@ -2097,7 +2138,38 @@
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
-      <c r="P38">
+      <c r="P38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update config tool, add base entity
</commit_message>
<xml_diff>
--- a/bin/resource/excel/entity_class.xlsx
+++ b/bin/resource/excel/entity_class.xlsx
@@ -24,7 +24,7 @@
     <author>1</author>
   </authors>
   <commentList>
-    <comment ref="C25" authorId="0" shapeId="0">
+    <comment ref="C26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="122">
   <si>
     <t>class</t>
   </si>
@@ -411,10 +411,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>Player</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>m</t>
     </r>
@@ -449,6 +445,81 @@
   </si>
   <si>
     <t>当前副本id</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>parent_class</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aseEntity</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>lass_name</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tring</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>类名</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Base</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entity</t>
+    </r>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -891,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -903,17 +974,19 @@
     <col min="2" max="2" width="19.375" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="20.375" customWidth="1"/>
-    <col min="5" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="18.25" customWidth="1"/>
-    <col min="9" max="9" width="19.125" customWidth="1"/>
-    <col min="10" max="12" width="10.875" customWidth="1"/>
-    <col min="13" max="13" width="10.375" customWidth="1"/>
-    <col min="14" max="14" width="11.5" customWidth="1"/>
-    <col min="15" max="15" width="10.875" customWidth="1"/>
-    <col min="16" max="16" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="10" max="10" width="19.125" customWidth="1"/>
+    <col min="11" max="13" width="10.875" customWidth="1"/>
+    <col min="14" max="14" width="10.375" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="10.875" customWidth="1"/>
+    <col min="17" max="17" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,50 +1003,50 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="E2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="I2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>109</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -982,9 +1055,12 @@
       <c r="O2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="P2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q2" s="6"/>
+    </row>
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1000,1176 +1076,1261 @@
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>30</v>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4">
-        <v>1</v>
-      </c>
+      <c r="J4" s="4"/>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="5"/>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" s="3">
-        <v>1</v>
-      </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P4" s="4"/>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3">
+      <c r="F7" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7">
         <v>1</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7">
+        <v>0</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P7" s="4"/>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="3">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
+        <v>38</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="5"/>
+      <c r="K9">
         <v>1</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4"/>
+      <c r="F10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P10" s="4"/>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>116</v>
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="9">
-        <v>1</v>
-      </c>
-      <c r="K11" s="9">
+      <c r="F11" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P11" s="4"/>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="3">
-        <v>1</v>
-      </c>
+      <c r="F12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" s="4"/>
       <c r="K12" s="3">
         <v>1</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="4"/>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P12" s="4"/>
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13" s="4"/>
+      <c r="F13" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P13" s="4"/>
+      <c r="Q13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="3">
-        <v>1</v>
-      </c>
-      <c r="K14" s="3">
+      <c r="F14" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14">
         <v>1</v>
       </c>
       <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P14" s="4"/>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4"/>
+      <c r="F15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="P15" s="4"/>
+      <c r="Q15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="3">
-        <v>1</v>
-      </c>
-      <c r="K16" s="3">
+      <c r="F16" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16">
         <v>1</v>
       </c>
       <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P16" s="4"/>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="4"/>
+      <c r="F17" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P17" s="4"/>
+      <c r="Q17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="3">
-        <v>1</v>
-      </c>
-      <c r="K18" s="3">
+      <c r="F18" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18">
         <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P18" s="4"/>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="4"/>
+      <c r="F19" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P19" s="4"/>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>111</v>
+      <c r="D20" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="3">
-        <v>1</v>
-      </c>
-      <c r="K20" s="3">
+      <c r="F20" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20">
         <v>1</v>
       </c>
       <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P20" s="4"/>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>65</v>
+      <c r="D21" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="4"/>
+      <c r="F21" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P21" s="4"/>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="D22" t="s">
-        <v>67</v>
+      <c r="D22" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="3">
-        <v>1</v>
-      </c>
-      <c r="K22" s="3">
+      <c r="F22" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22">
         <v>1</v>
       </c>
       <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P22" s="4"/>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="4"/>
+      <c r="F23" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="3">
+        <v>1</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-      <c r="P23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P23" s="4"/>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
         <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="3">
-        <v>1</v>
-      </c>
-      <c r="K24" s="3">
+      <c r="F24" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24">
         <v>1</v>
       </c>
       <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P24" s="4"/>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
-        <v>72</v>
+      <c r="B25" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="G25" t="s">
-        <v>75</v>
-      </c>
-      <c r="I25" s="4"/>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25" s="4"/>
+      <c r="F25" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="3">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-      <c r="P25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P25" s="4"/>
+      <c r="Q25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="G26" t="s">
-        <v>79</v>
-      </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="3">
-        <v>1</v>
-      </c>
-      <c r="K26" s="3">
+      <c r="F26" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26">
         <v>1</v>
       </c>
       <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
-      <c r="P26" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P26" s="4"/>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
         <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="G27" t="s">
-        <v>82</v>
-      </c>
-      <c r="I27" s="4"/>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27" s="4"/>
+      <c r="F27" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-      <c r="P27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P27" s="4"/>
+      <c r="Q27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28">
-        <v>1</v>
-      </c>
+      <c r="F28" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28" s="4"/>
       <c r="K28">
         <v>1</v>
       </c>
       <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P28" s="4"/>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>112</v>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="3">
-        <v>1</v>
-      </c>
-      <c r="K29" s="3">
+      <c r="J29" s="4"/>
+      <c r="K29">
         <v>1</v>
       </c>
       <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P29" s="4"/>
+      <c r="Q29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>79</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" t="s">
-        <v>40</v>
+        <v>85</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="3">
+        <v>1</v>
+      </c>
+      <c r="L30" s="3">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-      <c r="P30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P30" s="4"/>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>79</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="3">
-        <v>1</v>
-      </c>
-      <c r="K31" s="3">
+      <c r="J31" s="4"/>
+      <c r="K31">
         <v>1</v>
       </c>
       <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-      <c r="P31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P31" s="4"/>
+      <c r="Q31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>79</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="3">
+        <v>1</v>
+      </c>
+      <c r="L32" s="3">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
-      <c r="P32" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P32" s="4"/>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>79</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
         <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33">
-        <v>1</v>
-      </c>
+      <c r="J33" s="4"/>
       <c r="K33">
         <v>1</v>
       </c>
       <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P33" s="4"/>
+      <c r="Q33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34">
-        <v>1</v>
-      </c>
+      <c r="J34" s="4"/>
       <c r="K34">
         <v>1</v>
       </c>
       <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P34" s="4"/>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>112</v>
+        <v>83</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35">
-        <v>1</v>
-      </c>
+      <c r="J35" s="4"/>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="L35">
         <v>1</v>
       </c>
-      <c r="M35" s="4"/>
+      <c r="M35">
+        <v>0</v>
+      </c>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P35" s="4"/>
+      <c r="Q35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" t="s">
-        <v>99</v>
+        <v>85</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36">
-        <v>0</v>
-      </c>
+      <c r="J36" s="4"/>
       <c r="K36">
         <v>1</v>
       </c>
       <c r="L36">
         <v>1</v>
       </c>
-      <c r="M36" s="4"/>
+      <c r="M36">
+        <v>1</v>
+      </c>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P36" s="4"/>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
         <v>99</v>
       </c>
       <c r="D37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37">
-        <v>0</v>
-      </c>
+      <c r="J37" s="4"/>
       <c r="K37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37">
         <v>1</v>
       </c>
-      <c r="M37" s="4"/>
+      <c r="M37">
+        <v>1</v>
+      </c>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
-      <c r="P37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P37" s="4"/>
+      <c r="Q37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C38" t="s">
         <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38">
-        <v>0</v>
-      </c>
+      <c r="J38" s="4"/>
       <c r="K38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38">
         <v>1</v>
       </c>
-      <c r="M38" s="4"/>
+      <c r="M38">
+        <v>1</v>
+      </c>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
-      <c r="P38" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P38" s="4"/>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
         <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39">
-        <v>0</v>
-      </c>
+      <c r="J39" s="4"/>
       <c r="K39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39">
         <v>1</v>
       </c>
-      <c r="M39" s="4"/>
+      <c r="M39">
+        <v>1</v>
+      </c>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
-      <c r="P39">
+      <c r="P39" s="4"/>
+      <c r="Q39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new data management(unfinished)
</commit_message>
<xml_diff>
--- a/bin/resource/excel/entity_class.xlsx
+++ b/bin/resource/excel/entity_class.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -976,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add examples for container
</commit_message>
<xml_diff>
--- a/bin/resource/excel/entity_class.xlsx
+++ b/bin/resource/excel/entity_class.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\ARK\bin\resource\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\ark__\bin\resource\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDDAD3C-B13F-4646-A16C-E897276BCA29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DD8BF4-0BFD-4595-A0E9-CE9BBC3E896B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="145">
   <si>
     <t>class</t>
   </si>
@@ -277,9 +277,6 @@
     <t>穿戴的装备</t>
   </si>
   <si>
-    <t>EquipBag</t>
-  </si>
-  <si>
     <t>guid</t>
   </si>
   <si>
@@ -317,12 +314,6 @@
   </si>
   <si>
     <t>过期时间</t>
-  </si>
-  <si>
-    <t>装备的唯一id</t>
-  </si>
-  <si>
-    <t>装备配置id</t>
   </si>
   <si>
     <t>hp</t>
@@ -557,6 +548,70 @@
   </si>
   <si>
     <t>是否数据改变时发</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>equip_container</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_container</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备栏</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_bar_table</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillBarTable</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能栏</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能栏位置</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_id</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>int64</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能id</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>equip_bag_container</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备背包</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1010,17 +1065,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD7F117-52D8-42CE-8256-70EF3C94B5C3}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1034,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1052,13 +1108,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>8</v>
@@ -1070,30 +1126,30 @@
         <v>10</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -1109,7 +1165,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -1145,15 +1201,15 @@
         <v>24</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
@@ -1187,17 +1243,17 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F5" s="4"/>
       <c r="J5" s="9">
@@ -1221,17 +1277,17 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F6" s="4"/>
       <c r="J6">
@@ -1255,17 +1311,17 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F7" s="4"/>
       <c r="I7" s="4"/>
@@ -1293,13 +1349,13 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F8" s="4"/>
       <c r="I8" s="4"/>
@@ -1327,13 +1383,13 @@
         <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" t="s">
         <v>91</v>
-      </c>
-      <c r="E9" t="s">
-        <v>94</v>
       </c>
       <c r="F9" s="4"/>
       <c r="I9" s="4"/>
@@ -1361,13 +1417,13 @@
         <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F10" s="4"/>
       <c r="I10" s="4"/>
@@ -1395,13 +1451,13 @@
         <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F11" s="4"/>
       <c r="I11" s="4"/>
@@ -1432,25 +1488,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="7" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" customWidth="1"/>
-    <col min="10" max="12" width="10.88671875" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" customWidth="1"/>
-    <col min="16" max="17" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.36328125" customWidth="1"/>
+    <col min="6" max="7" width="11.453125" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="10" max="12" width="10.90625" customWidth="1"/>
+    <col min="13" max="13" width="10.36328125" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" customWidth="1"/>
+    <col min="15" max="15" width="10.90625" customWidth="1"/>
+    <col min="16" max="17" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1464,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1482,13 +1539,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>8</v>
@@ -1500,30 +1557,30 @@
         <v>10</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -1539,7 +1596,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -1575,10 +1632,10 @@
         <v>24</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1586,16 +1643,16 @@
         <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F4" s="4"/>
       <c r="I4" s="4"/>
@@ -1645,7 +1702,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
@@ -2071,7 +2128,7 @@
         <v>35</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F18" s="4"/>
       <c r="I18" s="4"/>
@@ -2105,7 +2162,7 @@
         <v>35</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F19" s="4"/>
       <c r="I19" s="4"/>
@@ -2272,10 +2329,10 @@
         <v>67</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E24" t="s">
         <v>68</v>
@@ -2309,10 +2366,10 @@
         <v>70</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E25" t="s">
         <v>71</v>
@@ -2338,18 +2395,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E26" t="s">
         <v>73</v>
@@ -2380,13 +2437,13 @@
         <v>72</v>
       </c>
       <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" t="s">
-        <v>76</v>
       </c>
       <c r="F27" s="4"/>
       <c r="I27" s="4"/>
@@ -2414,14 +2471,14 @@
         <v>72</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F28" s="4"/>
       <c r="I28" s="4"/>
@@ -2449,13 +2506,13 @@
         <v>72</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29" s="4"/>
       <c r="I29" s="4"/>
@@ -2483,13 +2540,13 @@
         <v>72</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
         <v>81</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>82</v>
-      </c>
-      <c r="E30" t="s">
-        <v>83</v>
       </c>
       <c r="F30" s="4"/>
       <c r="I30" s="4"/>
@@ -2517,13 +2574,13 @@
         <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31" s="4"/>
       <c r="I31" s="4"/>
@@ -2551,13 +2608,13 @@
         <v>72</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
         <v>35</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F32" s="4"/>
       <c r="I32" s="4"/>
@@ -2580,18 +2637,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" t="s">
-        <v>88</v>
+        <v>25</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="F33" s="4"/>
       <c r="I33" s="4"/>
@@ -2607,26 +2667,28 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" t="s">
-        <v>77</v>
+        <v>25</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" t="s">
-        <v>89</v>
+        <v>124</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="F34" s="4"/>
       <c r="I34" s="4"/>
@@ -2637,7 +2699,7 @@
         <v>1</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2646,6 +2708,148 @@
         <v>0</v>
       </c>
       <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
         <v>0</v>
       </c>
     </row>

</xml_diff>